<commit_message>
fix export jk missing item
</commit_message>
<xml_diff>
--- a/templates/template_form.xlsx
+++ b/templates/template_form.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="80">
   <si>
     <t>การไฟฟ้าส่วนภูมิภาค</t>
   </si>
@@ -267,6 +267,9 @@
   <si>
     <t>ค่าอุปกรณ์ ค่าขนส่ง ค่าติดตั้งและทดสอบ</t>
   </si>
+  <si>
+    <t>c</t>
+  </si>
 </sst>
 </file>
 
@@ -276,7 +279,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,6 +332,12 @@
       <sz val="22"/>
       <name val="TH SarabunPSK"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <name val="Webdings"/>
+      <family val="1"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -788,7 +797,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="366">
+  <cellXfs count="367">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1630,16 +1639,58 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="15" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1661,15 +1712,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1693,34 +1735,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1741,17 +1762,8 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1773,1311 +1785,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="24155400" y="21678900"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>281940</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectangle 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="24155400" y="21282660"/>
-          <a:ext cx="236220" cy="213360"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>281940</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="24170640" y="22029420"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="24170640" y="22410420"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>266700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="24155400" y="113088420"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>281940</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="Rectangle 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="24155400" y="112722660"/>
-          <a:ext cx="236220" cy="213360"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>274320</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="24170640" y="113827560"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>281940</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="24155400" y="113469420"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="24208740" y="116410740"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="Rectangle 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="24208740" y="116776500"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21968460" y="112753140"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21983700" y="116410740"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectangle 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21983700" y="116776500"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>266700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21960840" y="113454180"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21960840" y="113781840"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21960840" y="113118900"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectangle 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21968460" y="3025140"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>266700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21960840" y="3726180"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectangle 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21960840" y="4053840"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21960840" y="3390900"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21968460" y="21313140"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21983700" y="24970740"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>464820</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectangle 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21983700" y="25336500"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>266700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21960840" y="22014180"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21960840" y="22341840"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21960840" y="21678900"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectangle 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21968460" y="3025140"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>266700</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21960840" y="3726180"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Rectangle 10"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21960840" y="4053840"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>297180</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangle 9"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="21960840" y="3390900"/>
-          <a:ext cx="236220" cy="198120"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3348,8 +2055,8 @@
   </sheetPr>
   <dimension ref="A1:W101"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="50" zoomScaleNormal="55" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A58" zoomScale="50" zoomScaleNormal="55" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="P62" sqref="P62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="28.8" x14ac:dyDescent="0.55000000000000004"/>
@@ -3543,25 +2250,25 @@
       <c r="A7" s="106"/>
       <c r="B7" s="107"/>
       <c r="C7" s="108"/>
-      <c r="D7" s="326" t="s">
+      <c r="D7" s="357" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="327"/>
-      <c r="F7" s="327"/>
-      <c r="G7" s="327"/>
-      <c r="H7" s="328"/>
-      <c r="I7" s="326" t="s">
+      <c r="E7" s="358"/>
+      <c r="F7" s="358"/>
+      <c r="G7" s="358"/>
+      <c r="H7" s="359"/>
+      <c r="I7" s="357" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="328"/>
-      <c r="K7" s="326" t="s">
+      <c r="J7" s="359"/>
+      <c r="K7" s="357" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="328"/>
-      <c r="M7" s="326" t="s">
+      <c r="L7" s="359"/>
+      <c r="M7" s="357" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="328"/>
+      <c r="N7" s="359"/>
       <c r="O7" s="109"/>
       <c r="P7" s="107"/>
       <c r="Q7" s="109"/>
@@ -3655,7 +2362,9 @@
         <v>21</v>
       </c>
       <c r="O9" s="120"/>
-      <c r="P9" s="80"/>
+      <c r="P9" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q9" s="11" t="s">
         <v>22</v>
       </c>
@@ -3685,7 +2394,9 @@
       <c r="M10" s="324"/>
       <c r="N10" s="128"/>
       <c r="O10" s="129"/>
-      <c r="P10" s="80"/>
+      <c r="P10" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q10" s="11" t="s">
         <v>23</v>
       </c>
@@ -3720,7 +2431,9 @@
         <v>0</v>
       </c>
       <c r="O11" s="132"/>
-      <c r="P11" s="3"/>
+      <c r="P11" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q11" s="4" t="s">
         <v>24</v>
       </c>
@@ -3755,7 +2468,9 @@
         <v>0</v>
       </c>
       <c r="O12" s="134"/>
-      <c r="P12" s="3"/>
+      <c r="P12" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q12" s="4" t="s">
         <v>25</v>
       </c>
@@ -4880,10 +3595,10 @@
       <c r="D46" s="4"/>
       <c r="E46" s="167"/>
       <c r="F46" s="168"/>
-      <c r="G46" s="325" t="s">
+      <c r="G46" s="339" t="s">
         <v>28</v>
       </c>
-      <c r="H46" s="325"/>
+      <c r="H46" s="339"/>
       <c r="I46" s="169"/>
       <c r="J46" s="170"/>
       <c r="K46" s="171"/>
@@ -5006,30 +3721,30 @@
       <c r="V50" s="198"/>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="331" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="332"/>
-      <c r="C51" s="332"/>
-      <c r="D51" s="332"/>
-      <c r="E51" s="332"/>
-      <c r="F51" s="332"/>
-      <c r="G51" s="332"/>
-      <c r="H51" s="332"/>
-      <c r="I51" s="332"/>
-      <c r="J51" s="332"/>
-      <c r="K51" s="332"/>
-      <c r="L51" s="332"/>
-      <c r="M51" s="332"/>
-      <c r="N51" s="332"/>
-      <c r="O51" s="332"/>
-      <c r="P51" s="332"/>
-      <c r="Q51" s="332"/>
-      <c r="R51" s="332"/>
-      <c r="S51" s="332"/>
-      <c r="T51" s="332"/>
-      <c r="U51" s="332"/>
-      <c r="V51" s="333"/>
+      <c r="A51" s="345" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="346"/>
+      <c r="C51" s="346"/>
+      <c r="D51" s="346"/>
+      <c r="E51" s="346"/>
+      <c r="F51" s="346"/>
+      <c r="G51" s="346"/>
+      <c r="H51" s="346"/>
+      <c r="I51" s="346"/>
+      <c r="J51" s="346"/>
+      <c r="K51" s="346"/>
+      <c r="L51" s="346"/>
+      <c r="M51" s="346"/>
+      <c r="N51" s="346"/>
+      <c r="O51" s="346"/>
+      <c r="P51" s="346"/>
+      <c r="Q51" s="346"/>
+      <c r="R51" s="346"/>
+      <c r="S51" s="346"/>
+      <c r="T51" s="346"/>
+      <c r="U51" s="346"/>
+      <c r="V51" s="347"/>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="336" t="s">
@@ -5058,9 +3773,9 @@
       <c r="V52" s="338"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="339"/>
-      <c r="B53" s="340"/>
-      <c r="C53" s="340"/>
+      <c r="A53" s="350"/>
+      <c r="B53" s="351"/>
+      <c r="C53" s="351"/>
       <c r="D53" s="88"/>
       <c r="E53" s="88"/>
       <c r="F53" s="89"/>
@@ -5084,49 +3799,49 @@
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="341"/>
-      <c r="B54" s="342"/>
-      <c r="C54" s="342"/>
-      <c r="D54" s="342"/>
-      <c r="E54" s="342"/>
-      <c r="F54" s="342"/>
-      <c r="G54" s="342"/>
-      <c r="H54" s="342"/>
-      <c r="I54" s="342"/>
-      <c r="J54" s="342"/>
-      <c r="K54" s="342"/>
-      <c r="L54" s="342"/>
-      <c r="M54" s="342"/>
-      <c r="N54" s="342"/>
-      <c r="O54" s="342"/>
-      <c r="P54" s="342"/>
-      <c r="Q54" s="342"/>
-      <c r="R54" s="342"/>
-      <c r="S54" s="342"/>
-      <c r="T54" s="342"/>
-      <c r="U54" s="342"/>
-      <c r="V54" s="343"/>
+      <c r="A54" s="352"/>
+      <c r="B54" s="353"/>
+      <c r="C54" s="353"/>
+      <c r="D54" s="353"/>
+      <c r="E54" s="353"/>
+      <c r="F54" s="353"/>
+      <c r="G54" s="353"/>
+      <c r="H54" s="353"/>
+      <c r="I54" s="353"/>
+      <c r="J54" s="353"/>
+      <c r="K54" s="353"/>
+      <c r="L54" s="353"/>
+      <c r="M54" s="353"/>
+      <c r="N54" s="353"/>
+      <c r="O54" s="353"/>
+      <c r="P54" s="353"/>
+      <c r="Q54" s="353"/>
+      <c r="R54" s="353"/>
+      <c r="S54" s="353"/>
+      <c r="T54" s="353"/>
+      <c r="U54" s="353"/>
+      <c r="V54" s="354"/>
     </row>
     <row r="55" spans="1:22" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="344"/>
-      <c r="B55" s="345"/>
-      <c r="C55" s="345"/>
-      <c r="D55" s="345"/>
-      <c r="E55" s="345"/>
-      <c r="F55" s="345"/>
-      <c r="G55" s="345"/>
-      <c r="H55" s="345"/>
-      <c r="I55" s="345"/>
-      <c r="J55" s="345"/>
-      <c r="K55" s="345"/>
-      <c r="L55" s="345"/>
-      <c r="M55" s="345"/>
-      <c r="N55" s="345"/>
-      <c r="O55" s="345"/>
-      <c r="P55" s="345"/>
-      <c r="Q55" s="345"/>
-      <c r="R55" s="345"/>
-      <c r="S55" s="345"/>
+      <c r="A55" s="355"/>
+      <c r="B55" s="356"/>
+      <c r="C55" s="356"/>
+      <c r="D55" s="356"/>
+      <c r="E55" s="356"/>
+      <c r="F55" s="356"/>
+      <c r="G55" s="356"/>
+      <c r="H55" s="356"/>
+      <c r="I55" s="356"/>
+      <c r="J55" s="356"/>
+      <c r="K55" s="356"/>
+      <c r="L55" s="356"/>
+      <c r="M55" s="356"/>
+      <c r="N55" s="356"/>
+      <c r="O55" s="356"/>
+      <c r="P55" s="356"/>
+      <c r="Q55" s="356"/>
+      <c r="R55" s="356"/>
+      <c r="S55" s="356"/>
       <c r="T55" s="87" t="s">
         <v>68</v>
       </c>
@@ -5165,25 +3880,25 @@
       <c r="A57" s="106"/>
       <c r="B57" s="107"/>
       <c r="C57" s="108"/>
-      <c r="D57" s="326" t="s">
+      <c r="D57" s="357" t="s">
         <v>7</v>
       </c>
-      <c r="E57" s="327"/>
-      <c r="F57" s="327"/>
-      <c r="G57" s="327"/>
-      <c r="H57" s="328"/>
-      <c r="I57" s="326" t="s">
+      <c r="E57" s="358"/>
+      <c r="F57" s="358"/>
+      <c r="G57" s="358"/>
+      <c r="H57" s="359"/>
+      <c r="I57" s="357" t="s">
         <v>8</v>
       </c>
-      <c r="J57" s="328"/>
-      <c r="K57" s="326" t="s">
+      <c r="J57" s="359"/>
+      <c r="K57" s="357" t="s">
         <v>9</v>
       </c>
-      <c r="L57" s="328"/>
-      <c r="M57" s="326" t="s">
+      <c r="L57" s="359"/>
+      <c r="M57" s="357" t="s">
         <v>10</v>
       </c>
-      <c r="N57" s="328"/>
+      <c r="N57" s="359"/>
       <c r="O57" s="109"/>
       <c r="P57" s="107"/>
       <c r="Q57" s="109"/>
@@ -5277,7 +3992,9 @@
         <v>21</v>
       </c>
       <c r="O59" s="120"/>
-      <c r="P59" s="80"/>
+      <c r="P59" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q59" s="11" t="s">
         <v>22</v>
       </c>
@@ -5312,7 +4029,9 @@
         <v>0</v>
       </c>
       <c r="O60" s="134"/>
-      <c r="P60" s="80"/>
+      <c r="P60" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q60" s="11" t="s">
         <v>23</v>
       </c>
@@ -5347,7 +4066,9 @@
         <v>0</v>
       </c>
       <c r="O61" s="134"/>
-      <c r="P61" s="3"/>
+      <c r="P61" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q61" s="4" t="s">
         <v>24</v>
       </c>
@@ -5382,7 +4103,9 @@
         <v>0</v>
       </c>
       <c r="O62" s="134"/>
-      <c r="P62" s="3"/>
+      <c r="P62" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q62" s="4" t="s">
         <v>25</v>
       </c>
@@ -5423,9 +4146,9 @@
       <c r="Q63" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="R63" s="334"/>
-      <c r="S63" s="334"/>
-      <c r="T63" s="334"/>
+      <c r="R63" s="348"/>
+      <c r="S63" s="348"/>
+      <c r="T63" s="348"/>
       <c r="U63" s="4" t="s">
         <v>28</v>
       </c>
@@ -5458,11 +4181,11 @@
       <c r="O64" s="134"/>
       <c r="P64" s="83"/>
       <c r="Q64" s="47"/>
-      <c r="R64" s="335" t="s">
+      <c r="R64" s="349" t="s">
         <v>66</v>
       </c>
-      <c r="S64" s="335"/>
-      <c r="T64" s="335"/>
+      <c r="S64" s="349"/>
+      <c r="T64" s="349"/>
       <c r="U64" s="4" t="s">
         <v>29</v>
       </c>
@@ -5668,7 +4391,9 @@
         <v>0</v>
       </c>
       <c r="O70" s="134"/>
-      <c r="P70" s="3"/>
+      <c r="P70" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q70" s="4" t="s">
         <v>41</v>
       </c>
@@ -5703,7 +4428,9 @@
         <v>0</v>
       </c>
       <c r="O71" s="134"/>
-      <c r="P71" s="3"/>
+      <c r="P71" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q71" s="4" t="s">
         <v>42</v>
       </c>
@@ -6556,10 +5283,10 @@
     </row>
     <row r="95" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="151"/>
-      <c r="B95" s="329" t="s">
+      <c r="B95" s="343" t="s">
         <v>37</v>
       </c>
-      <c r="C95" s="330"/>
+      <c r="C95" s="344"/>
       <c r="D95" s="154"/>
       <c r="E95" s="155"/>
       <c r="F95" s="156"/>
@@ -6624,15 +5351,15 @@
         <v>0</v>
       </c>
       <c r="O96" s="160"/>
-      <c r="P96" s="350" t="s">
+      <c r="P96" s="333" t="s">
         <v>59</v>
       </c>
-      <c r="Q96" s="351"/>
-      <c r="R96" s="351"/>
-      <c r="S96" s="351"/>
-      <c r="T96" s="351"/>
-      <c r="U96" s="351"/>
-      <c r="V96" s="352"/>
+      <c r="Q96" s="334"/>
+      <c r="R96" s="334"/>
+      <c r="S96" s="334"/>
+      <c r="T96" s="334"/>
+      <c r="U96" s="334"/>
+      <c r="V96" s="335"/>
     </row>
     <row r="97" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="336" t="s">
@@ -6643,10 +5370,10 @@
       <c r="D97" s="4"/>
       <c r="E97" s="167"/>
       <c r="F97" s="168"/>
-      <c r="G97" s="325" t="s">
+      <c r="G97" s="339" t="s">
         <v>28</v>
       </c>
-      <c r="H97" s="325"/>
+      <c r="H97" s="339"/>
       <c r="I97" s="169"/>
       <c r="J97" s="170"/>
       <c r="K97" s="171"/>
@@ -6668,9 +5395,9 @@
       <c r="V97" s="185"/>
     </row>
     <row r="98" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="353"/>
-      <c r="B98" s="346"/>
-      <c r="C98" s="354"/>
+      <c r="A98" s="340"/>
+      <c r="B98" s="329"/>
+      <c r="C98" s="341"/>
       <c r="D98" s="179"/>
       <c r="E98" s="179"/>
       <c r="F98" s="180"/>
@@ -6697,20 +5424,20 @@
       <c r="W98" s="185"/>
     </row>
     <row r="99" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="353" t="s">
+      <c r="A99" s="340" t="s">
         <v>33</v>
       </c>
-      <c r="B99" s="346"/>
-      <c r="C99" s="354"/>
+      <c r="B99" s="329"/>
+      <c r="C99" s="341"/>
       <c r="D99" s="4"/>
-      <c r="E99" s="355" t="s">
+      <c r="E99" s="342" t="s">
         <v>34</v>
       </c>
-      <c r="F99" s="355"/>
-      <c r="G99" s="355"/>
-      <c r="H99" s="355"/>
-      <c r="I99" s="355"/>
-      <c r="J99" s="355"/>
+      <c r="F99" s="342"/>
+      <c r="G99" s="342"/>
+      <c r="H99" s="342"/>
+      <c r="I99" s="342"/>
+      <c r="J99" s="342"/>
       <c r="K99" s="169"/>
       <c r="L99" s="182"/>
       <c r="M99" s="211"/>
@@ -6735,13 +5462,13 @@
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="177"/>
-      <c r="F100" s="346" t="s">
+      <c r="F100" s="329" t="s">
         <v>69</v>
       </c>
-      <c r="G100" s="346"/>
-      <c r="H100" s="346"/>
-      <c r="I100" s="346"/>
-      <c r="J100" s="346"/>
+      <c r="G100" s="329"/>
+      <c r="H100" s="329"/>
+      <c r="I100" s="329"/>
+      <c r="J100" s="329"/>
       <c r="K100" s="189"/>
       <c r="L100" s="190"/>
       <c r="M100" s="214"/>
@@ -6761,20 +5488,20 @@
       <c r="W100" s="149"/>
     </row>
     <row r="101" spans="1:23" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="347" t="s">
+      <c r="A101" s="330" t="s">
         <v>35</v>
       </c>
-      <c r="B101" s="348"/>
-      <c r="C101" s="349"/>
+      <c r="B101" s="331"/>
+      <c r="C101" s="332"/>
       <c r="D101" s="139"/>
       <c r="E101" s="87"/>
-      <c r="F101" s="348" t="s">
+      <c r="F101" s="331" t="s">
         <v>36</v>
       </c>
-      <c r="G101" s="348"/>
-      <c r="H101" s="348"/>
-      <c r="I101" s="348"/>
-      <c r="J101" s="348"/>
+      <c r="G101" s="331"/>
+      <c r="H101" s="331"/>
+      <c r="I101" s="331"/>
+      <c r="J101" s="331"/>
       <c r="K101" s="193"/>
       <c r="L101" s="194"/>
       <c r="M101" s="218"/>
@@ -6790,15 +5517,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="F100:J100"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="F101:J101"/>
-    <mergeCell ref="P96:V96"/>
-    <mergeCell ref="A97:C97"/>
-    <mergeCell ref="G97:H97"/>
-    <mergeCell ref="A98:C98"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="E99:J99"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
     <mergeCell ref="B95:C95"/>
     <mergeCell ref="A51:V51"/>
     <mergeCell ref="R63:T63"/>
@@ -6811,11 +5534,15 @@
     <mergeCell ref="I57:J57"/>
     <mergeCell ref="K57:L57"/>
     <mergeCell ref="M57:N57"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="F100:J100"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="F101:J101"/>
+    <mergeCell ref="P96:V96"/>
+    <mergeCell ref="A97:C97"/>
+    <mergeCell ref="G97:H97"/>
+    <mergeCell ref="A98:C98"/>
+    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="E99:J99"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.31496062992126" right="0.31496062992126" top="0.59055118110236204" bottom="0.59055118110236204" header="0.31496062992126" footer="0.31496062992126"/>
@@ -6823,7 +5550,6 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="50" max="16383" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6834,8 +5560,8 @@
   </sheetPr>
   <dimension ref="A1:V103"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="50" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A59" zoomScale="50" zoomScaleNormal="100" zoomScaleSheetLayoutView="50" workbookViewId="0">
+      <selection activeCell="P70" sqref="P70:P71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="28.8" x14ac:dyDescent="0.55000000000000004"/>
@@ -6916,9 +5642,9 @@
       <c r="V2" s="277"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="339"/>
-      <c r="B3" s="340"/>
-      <c r="C3" s="340"/>
+      <c r="A3" s="350"/>
+      <c r="B3" s="351"/>
+      <c r="C3" s="351"/>
       <c r="D3" s="224"/>
       <c r="E3" s="224"/>
       <c r="F3" s="89"/>
@@ -7031,25 +5757,25 @@
       <c r="A7" s="106"/>
       <c r="B7" s="107"/>
       <c r="C7" s="108"/>
-      <c r="D7" s="326" t="s">
+      <c r="D7" s="357" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="327"/>
-      <c r="F7" s="327"/>
-      <c r="G7" s="327"/>
-      <c r="H7" s="328"/>
-      <c r="I7" s="356" t="s">
+      <c r="E7" s="358"/>
+      <c r="F7" s="358"/>
+      <c r="G7" s="358"/>
+      <c r="H7" s="359"/>
+      <c r="I7" s="360" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="357"/>
-      <c r="K7" s="356" t="s">
+      <c r="J7" s="361"/>
+      <c r="K7" s="360" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="357"/>
-      <c r="M7" s="326" t="s">
+      <c r="L7" s="361"/>
+      <c r="M7" s="357" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="328"/>
+      <c r="N7" s="359"/>
       <c r="O7" s="109"/>
       <c r="P7" s="107"/>
       <c r="Q7" s="109"/>
@@ -7073,10 +5799,10 @@
       <c r="E8" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="358" t="s">
+      <c r="F8" s="362" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="359"/>
+      <c r="G8" s="363"/>
       <c r="H8" s="114" t="s">
         <v>16</v>
       </c>
@@ -7119,10 +5845,10 @@
       <c r="C9" s="121"/>
       <c r="D9" s="119"/>
       <c r="E9" s="119"/>
-      <c r="F9" s="360" t="s">
+      <c r="F9" s="364" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="361"/>
+      <c r="G9" s="365"/>
       <c r="H9" s="122" t="s">
         <v>21</v>
       </c>
@@ -7139,7 +5865,9 @@
         <v>21</v>
       </c>
       <c r="O9" s="120"/>
-      <c r="P9" s="80"/>
+      <c r="P9" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q9" s="11" t="s">
         <v>22</v>
       </c>
@@ -7172,7 +5900,9 @@
         <v>0</v>
       </c>
       <c r="O10" s="235"/>
-      <c r="P10" s="80"/>
+      <c r="P10" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q10" s="11" t="s">
         <v>23</v>
       </c>
@@ -7205,7 +5935,9 @@
         <v>0</v>
       </c>
       <c r="O11" s="240"/>
-      <c r="P11" s="3"/>
+      <c r="P11" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q11" s="4" t="s">
         <v>24</v>
       </c>
@@ -7238,7 +5970,9 @@
         <v>0</v>
       </c>
       <c r="O12" s="242"/>
-      <c r="P12" s="3"/>
+      <c r="P12" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q12" s="4" t="s">
         <v>25</v>
       </c>
@@ -8299,10 +7033,10 @@
       <c r="D46" s="4"/>
       <c r="E46" s="167"/>
       <c r="F46" s="168"/>
-      <c r="G46" s="325" t="s">
+      <c r="G46" s="339" t="s">
         <v>28</v>
       </c>
-      <c r="H46" s="325"/>
+      <c r="H46" s="339"/>
       <c r="I46" s="169"/>
       <c r="J46" s="170"/>
       <c r="K46" s="171"/>
@@ -8426,30 +7160,30 @@
       <c r="V50" s="198"/>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="331" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="332"/>
-      <c r="C51" s="332"/>
-      <c r="D51" s="332"/>
-      <c r="E51" s="332"/>
-      <c r="F51" s="332"/>
-      <c r="G51" s="332"/>
-      <c r="H51" s="332"/>
-      <c r="I51" s="332"/>
-      <c r="J51" s="332"/>
-      <c r="K51" s="332"/>
-      <c r="L51" s="332"/>
-      <c r="M51" s="332"/>
-      <c r="N51" s="332"/>
-      <c r="O51" s="332"/>
-      <c r="P51" s="332"/>
-      <c r="Q51" s="332"/>
-      <c r="R51" s="332"/>
-      <c r="S51" s="332"/>
-      <c r="T51" s="332"/>
-      <c r="U51" s="332"/>
-      <c r="V51" s="333"/>
+      <c r="A51" s="345" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="346"/>
+      <c r="C51" s="346"/>
+      <c r="D51" s="346"/>
+      <c r="E51" s="346"/>
+      <c r="F51" s="346"/>
+      <c r="G51" s="346"/>
+      <c r="H51" s="346"/>
+      <c r="I51" s="346"/>
+      <c r="J51" s="346"/>
+      <c r="K51" s="346"/>
+      <c r="L51" s="346"/>
+      <c r="M51" s="346"/>
+      <c r="N51" s="346"/>
+      <c r="O51" s="346"/>
+      <c r="P51" s="346"/>
+      <c r="Q51" s="346"/>
+      <c r="R51" s="346"/>
+      <c r="S51" s="346"/>
+      <c r="T51" s="346"/>
+      <c r="U51" s="346"/>
+      <c r="V51" s="347"/>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="336" t="s">
@@ -8478,9 +7212,9 @@
       <c r="V52" s="338"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="339"/>
-      <c r="B53" s="340"/>
-      <c r="C53" s="340"/>
+      <c r="A53" s="350"/>
+      <c r="B53" s="351"/>
+      <c r="C53" s="351"/>
       <c r="D53" s="224"/>
       <c r="E53" s="224"/>
       <c r="F53" s="89"/>
@@ -8504,49 +7238,49 @@
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="341"/>
-      <c r="B54" s="342"/>
-      <c r="C54" s="342"/>
-      <c r="D54" s="342"/>
-      <c r="E54" s="342"/>
-      <c r="F54" s="342"/>
-      <c r="G54" s="342"/>
-      <c r="H54" s="342"/>
-      <c r="I54" s="342"/>
-      <c r="J54" s="342"/>
-      <c r="K54" s="342"/>
-      <c r="L54" s="342"/>
-      <c r="M54" s="342"/>
-      <c r="N54" s="342"/>
-      <c r="O54" s="342"/>
-      <c r="P54" s="342"/>
-      <c r="Q54" s="342"/>
-      <c r="R54" s="342"/>
-      <c r="S54" s="342"/>
-      <c r="T54" s="342"/>
-      <c r="U54" s="342"/>
-      <c r="V54" s="343"/>
+      <c r="A54" s="352"/>
+      <c r="B54" s="353"/>
+      <c r="C54" s="353"/>
+      <c r="D54" s="353"/>
+      <c r="E54" s="353"/>
+      <c r="F54" s="353"/>
+      <c r="G54" s="353"/>
+      <c r="H54" s="353"/>
+      <c r="I54" s="353"/>
+      <c r="J54" s="353"/>
+      <c r="K54" s="353"/>
+      <c r="L54" s="353"/>
+      <c r="M54" s="353"/>
+      <c r="N54" s="353"/>
+      <c r="O54" s="353"/>
+      <c r="P54" s="353"/>
+      <c r="Q54" s="353"/>
+      <c r="R54" s="353"/>
+      <c r="S54" s="353"/>
+      <c r="T54" s="353"/>
+      <c r="U54" s="353"/>
+      <c r="V54" s="354"/>
     </row>
     <row r="55" spans="1:22" ht="56.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="344"/>
-      <c r="B55" s="345"/>
-      <c r="C55" s="345"/>
-      <c r="D55" s="345"/>
-      <c r="E55" s="345"/>
-      <c r="F55" s="345"/>
-      <c r="G55" s="345"/>
-      <c r="H55" s="345"/>
-      <c r="I55" s="345"/>
-      <c r="J55" s="345"/>
-      <c r="K55" s="345"/>
-      <c r="L55" s="345"/>
-      <c r="M55" s="345"/>
-      <c r="N55" s="345"/>
-      <c r="O55" s="345"/>
-      <c r="P55" s="345"/>
-      <c r="Q55" s="345"/>
-      <c r="R55" s="345"/>
-      <c r="S55" s="345"/>
+      <c r="A55" s="355"/>
+      <c r="B55" s="356"/>
+      <c r="C55" s="356"/>
+      <c r="D55" s="356"/>
+      <c r="E55" s="356"/>
+      <c r="F55" s="356"/>
+      <c r="G55" s="356"/>
+      <c r="H55" s="356"/>
+      <c r="I55" s="356"/>
+      <c r="J55" s="356"/>
+      <c r="K55" s="356"/>
+      <c r="L55" s="356"/>
+      <c r="M55" s="356"/>
+      <c r="N55" s="356"/>
+      <c r="O55" s="356"/>
+      <c r="P55" s="356"/>
+      <c r="Q55" s="356"/>
+      <c r="R55" s="356"/>
+      <c r="S55" s="356"/>
       <c r="T55" s="87" t="s">
         <v>3</v>
       </c>
@@ -8585,25 +7319,25 @@
       <c r="A57" s="106"/>
       <c r="B57" s="107"/>
       <c r="C57" s="108"/>
-      <c r="D57" s="326" t="s">
+      <c r="D57" s="357" t="s">
         <v>7</v>
       </c>
-      <c r="E57" s="327"/>
-      <c r="F57" s="327"/>
-      <c r="G57" s="327"/>
-      <c r="H57" s="328"/>
-      <c r="I57" s="356" t="s">
+      <c r="E57" s="358"/>
+      <c r="F57" s="358"/>
+      <c r="G57" s="358"/>
+      <c r="H57" s="359"/>
+      <c r="I57" s="360" t="s">
         <v>8</v>
       </c>
-      <c r="J57" s="357"/>
-      <c r="K57" s="356" t="s">
+      <c r="J57" s="361"/>
+      <c r="K57" s="360" t="s">
         <v>9</v>
       </c>
-      <c r="L57" s="357"/>
-      <c r="M57" s="326" t="s">
+      <c r="L57" s="361"/>
+      <c r="M57" s="357" t="s">
         <v>10</v>
       </c>
-      <c r="N57" s="328"/>
+      <c r="N57" s="359"/>
       <c r="O57" s="109"/>
       <c r="P57" s="107"/>
       <c r="Q57" s="109"/>
@@ -8627,10 +7361,10 @@
       <c r="E58" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="F58" s="358" t="s">
+      <c r="F58" s="362" t="s">
         <v>15</v>
       </c>
-      <c r="G58" s="359"/>
+      <c r="G58" s="363"/>
       <c r="H58" s="114" t="s">
         <v>16</v>
       </c>
@@ -8673,10 +7407,10 @@
       <c r="C59" s="121"/>
       <c r="D59" s="119"/>
       <c r="E59" s="119"/>
-      <c r="F59" s="360" t="s">
+      <c r="F59" s="364" t="s">
         <v>20</v>
       </c>
-      <c r="G59" s="361"/>
+      <c r="G59" s="365"/>
       <c r="H59" s="122" t="s">
         <v>21</v>
       </c>
@@ -8693,7 +7427,9 @@
         <v>21</v>
       </c>
       <c r="O59" s="120"/>
-      <c r="P59" s="80"/>
+      <c r="P59" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q59" s="11" t="s">
         <v>22</v>
       </c>
@@ -8726,7 +7462,9 @@
         <v>0</v>
       </c>
       <c r="O60" s="235"/>
-      <c r="P60" s="80"/>
+      <c r="P60" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q60" s="11" t="s">
         <v>23</v>
       </c>
@@ -8759,7 +7497,9 @@
         <v>0</v>
       </c>
       <c r="O61" s="242"/>
-      <c r="P61" s="3"/>
+      <c r="P61" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q61" s="4" t="s">
         <v>24</v>
       </c>
@@ -8792,7 +7532,9 @@
         <v>0</v>
       </c>
       <c r="O62" s="242"/>
-      <c r="P62" s="3"/>
+      <c r="P62" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q62" s="4" t="s">
         <v>25</v>
       </c>
@@ -8831,9 +7573,9 @@
       <c r="Q63" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="R63" s="334"/>
-      <c r="S63" s="334"/>
-      <c r="T63" s="334"/>
+      <c r="R63" s="348"/>
+      <c r="S63" s="348"/>
+      <c r="T63" s="348"/>
       <c r="U63" s="4" t="s">
         <v>28</v>
       </c>
@@ -8864,12 +7606,12 @@
       <c r="O64" s="242"/>
       <c r="P64" s="83"/>
       <c r="Q64" s="47"/>
-      <c r="R64" s="335" t="str">
+      <c r="R64" s="349" t="str">
         <f>+R14</f>
         <v>( นาย... )</v>
       </c>
-      <c r="S64" s="335"/>
-      <c r="T64" s="335"/>
+      <c r="S64" s="349"/>
+      <c r="T64" s="349"/>
       <c r="U64" s="4" t="s">
         <v>29</v>
       </c>
@@ -9063,7 +7805,9 @@
         <v>0</v>
       </c>
       <c r="O70" s="242"/>
-      <c r="P70" s="3"/>
+      <c r="P70" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q70" s="4" t="s">
         <v>41</v>
       </c>
@@ -9096,7 +7840,9 @@
         <v>0</v>
       </c>
       <c r="O71" s="242"/>
-      <c r="P71" s="3"/>
+      <c r="P71" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="Q71" s="4" t="s">
         <v>42</v>
       </c>
@@ -9904,10 +8650,10 @@
     </row>
     <row r="95" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="151"/>
-      <c r="B95" s="329" t="s">
+      <c r="B95" s="343" t="s">
         <v>37</v>
       </c>
-      <c r="C95" s="330"/>
+      <c r="C95" s="344"/>
       <c r="D95" s="154"/>
       <c r="E95" s="155"/>
       <c r="F95" s="156"/>
@@ -9972,15 +8718,15 @@
         <v>0</v>
       </c>
       <c r="O96" s="160"/>
-      <c r="P96" s="350" t="s">
+      <c r="P96" s="333" t="s">
         <v>59</v>
       </c>
-      <c r="Q96" s="351"/>
-      <c r="R96" s="351"/>
-      <c r="S96" s="351"/>
-      <c r="T96" s="351"/>
-      <c r="U96" s="351"/>
-      <c r="V96" s="352"/>
+      <c r="Q96" s="334"/>
+      <c r="R96" s="334"/>
+      <c r="S96" s="334"/>
+      <c r="T96" s="334"/>
+      <c r="U96" s="334"/>
+      <c r="V96" s="335"/>
     </row>
     <row r="97" spans="1:22" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="336" t="s">
@@ -9991,10 +8737,10 @@
       <c r="D97" s="4"/>
       <c r="E97" s="167"/>
       <c r="F97" s="168"/>
-      <c r="G97" s="325" t="s">
+      <c r="G97" s="339" t="s">
         <v>28</v>
       </c>
-      <c r="H97" s="325"/>
+      <c r="H97" s="339"/>
       <c r="I97" s="180"/>
       <c r="J97" s="170"/>
       <c r="K97" s="170"/>
@@ -10016,9 +8762,9 @@
       <c r="V97" s="185"/>
     </row>
     <row r="98" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="353"/>
-      <c r="B98" s="346"/>
-      <c r="C98" s="354"/>
+      <c r="A98" s="340"/>
+      <c r="B98" s="329"/>
+      <c r="C98" s="341"/>
       <c r="D98" s="179"/>
       <c r="E98" s="179"/>
       <c r="F98" s="180"/>
@@ -10044,20 +8790,20 @@
       <c r="V98" s="185"/>
     </row>
     <row r="99" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="353" t="s">
+      <c r="A99" s="340" t="s">
         <v>33</v>
       </c>
-      <c r="B99" s="346"/>
-      <c r="C99" s="354"/>
+      <c r="B99" s="329"/>
+      <c r="C99" s="341"/>
       <c r="D99" s="4"/>
-      <c r="E99" s="355" t="s">
+      <c r="E99" s="342" t="s">
         <v>34</v>
       </c>
-      <c r="F99" s="355"/>
-      <c r="G99" s="355"/>
-      <c r="H99" s="355"/>
-      <c r="I99" s="355"/>
-      <c r="J99" s="355"/>
+      <c r="F99" s="342"/>
+      <c r="G99" s="342"/>
+      <c r="H99" s="342"/>
+      <c r="I99" s="342"/>
+      <c r="J99" s="342"/>
       <c r="K99" s="181"/>
       <c r="L99" s="250"/>
       <c r="M99" s="251"/>
@@ -10074,19 +8820,19 @@
       <c r="V99" s="185"/>
     </row>
     <row r="100" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100" s="353"/>
-      <c r="B100" s="346"/>
-      <c r="C100" s="354"/>
+      <c r="A100" s="340"/>
+      <c r="B100" s="329"/>
+      <c r="C100" s="341"/>
       <c r="D100" s="4"/>
-      <c r="E100" s="346" t="str">
+      <c r="E100" s="329" t="str">
         <f>+F49</f>
         <v>( นาย... ) ตำแหน่ง กบศ.</v>
       </c>
-      <c r="F100" s="346"/>
-      <c r="G100" s="346"/>
-      <c r="H100" s="346"/>
-      <c r="I100" s="346"/>
-      <c r="J100" s="346"/>
+      <c r="F100" s="329"/>
+      <c r="G100" s="329"/>
+      <c r="H100" s="329"/>
+      <c r="I100" s="329"/>
+      <c r="J100" s="329"/>
       <c r="K100" s="254"/>
       <c r="L100" s="255"/>
       <c r="M100" s="256"/>
@@ -10105,20 +8851,20 @@
       <c r="V100" s="217"/>
     </row>
     <row r="101" spans="1:22" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="347" t="s">
+      <c r="A101" s="330" t="s">
         <v>35</v>
       </c>
-      <c r="B101" s="348"/>
-      <c r="C101" s="349"/>
+      <c r="B101" s="331"/>
+      <c r="C101" s="332"/>
       <c r="D101" s="139"/>
       <c r="E101" s="87"/>
-      <c r="F101" s="348" t="s">
+      <c r="F101" s="331" t="s">
         <v>36</v>
       </c>
-      <c r="G101" s="348"/>
-      <c r="H101" s="348"/>
-      <c r="I101" s="348"/>
-      <c r="J101" s="348"/>
+      <c r="G101" s="331"/>
+      <c r="H101" s="331"/>
+      <c r="I101" s="331"/>
+      <c r="J101" s="331"/>
       <c r="K101" s="258"/>
       <c r="L101" s="259"/>
       <c r="M101" s="260"/>
@@ -10152,22 +8898,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="A98:C98"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="P96:V96"/>
-    <mergeCell ref="A97:C97"/>
-    <mergeCell ref="G97:H97"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="E99:J99"/>
-    <mergeCell ref="A100:C100"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="F101:J101"/>
-    <mergeCell ref="E100:J100"/>
-    <mergeCell ref="A55:S55"/>
-    <mergeCell ref="D57:H57"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="M57:N57"/>
     <mergeCell ref="R64:T64"/>
     <mergeCell ref="A51:V51"/>
     <mergeCell ref="A52:V52"/>
@@ -10184,13 +8914,28 @@
     <mergeCell ref="F59:G59"/>
     <mergeCell ref="R63:T63"/>
     <mergeCell ref="A54:V54"/>
+    <mergeCell ref="A55:S55"/>
+    <mergeCell ref="D57:H57"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="M57:N57"/>
+    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="E99:J99"/>
+    <mergeCell ref="A100:C100"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="F101:J101"/>
+    <mergeCell ref="E100:J100"/>
+    <mergeCell ref="A98:C98"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="P96:V96"/>
+    <mergeCell ref="A97:C97"/>
+    <mergeCell ref="G97:H97"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="30" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="50" max="16383" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -10199,7 +8944,7 @@
   <dimension ref="A1:X103"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="53" zoomScaleNormal="100" zoomScaleSheetLayoutView="53" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:H44"/>
+      <selection activeCell="R9" sqref="R9:R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="28.8" x14ac:dyDescent="0.55000000000000004"/>
@@ -10286,9 +9031,9 @@
       <c r="X2" s="277"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="339"/>
-      <c r="B3" s="340"/>
-      <c r="C3" s="340"/>
+      <c r="A3" s="350"/>
+      <c r="B3" s="351"/>
+      <c r="C3" s="351"/>
       <c r="D3" s="224"/>
       <c r="E3" s="224"/>
       <c r="F3" s="224"/>
@@ -10409,27 +9154,27 @@
       <c r="A7" s="106"/>
       <c r="B7" s="107"/>
       <c r="C7" s="108"/>
-      <c r="D7" s="326" t="s">
+      <c r="D7" s="357" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="327"/>
-      <c r="F7" s="327"/>
-      <c r="G7" s="327"/>
-      <c r="H7" s="327"/>
-      <c r="I7" s="327"/>
-      <c r="J7" s="328"/>
-      <c r="K7" s="356" t="s">
+      <c r="E7" s="358"/>
+      <c r="F7" s="358"/>
+      <c r="G7" s="358"/>
+      <c r="H7" s="358"/>
+      <c r="I7" s="358"/>
+      <c r="J7" s="359"/>
+      <c r="K7" s="360" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="357"/>
-      <c r="M7" s="356" t="s">
+      <c r="L7" s="361"/>
+      <c r="M7" s="360" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="357"/>
-      <c r="O7" s="326" t="s">
+      <c r="N7" s="361"/>
+      <c r="O7" s="357" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="328"/>
+      <c r="P7" s="359"/>
       <c r="Q7" s="109"/>
       <c r="R7" s="107"/>
       <c r="S7" s="109"/>
@@ -10459,10 +9204,10 @@
       <c r="G8" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="358" t="s">
+      <c r="H8" s="362" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="359"/>
+      <c r="I8" s="363"/>
       <c r="J8" s="114" t="s">
         <v>16</v>
       </c>
@@ -10511,10 +9256,10 @@
       <c r="G9" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="360" t="s">
+      <c r="H9" s="364" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="361"/>
+      <c r="I9" s="365"/>
       <c r="J9" s="122" t="s">
         <v>21</v>
       </c>
@@ -10531,7 +9276,9 @@
         <v>21</v>
       </c>
       <c r="Q9" s="120"/>
-      <c r="R9" s="80"/>
+      <c r="R9" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="S9" s="11" t="s">
         <v>22</v>
       </c>
@@ -10549,7 +9296,7 @@
       <c r="E10" s="58"/>
       <c r="F10" s="73"/>
       <c r="G10" s="73"/>
-      <c r="H10" s="362"/>
+      <c r="H10" s="325"/>
       <c r="I10" s="232"/>
       <c r="J10" s="233"/>
       <c r="K10" s="234"/>
@@ -10569,7 +9316,9 @@
         <v>0</v>
       </c>
       <c r="Q10" s="235"/>
-      <c r="R10" s="80"/>
+      <c r="R10" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="S10" s="11" t="s">
         <v>23</v>
       </c>
@@ -10587,7 +9336,7 @@
       <c r="E11" s="9"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
-      <c r="H11" s="363"/>
+      <c r="H11" s="326"/>
       <c r="I11" s="202"/>
       <c r="J11" s="237"/>
       <c r="K11" s="238"/>
@@ -10607,7 +9356,9 @@
         <v>0</v>
       </c>
       <c r="Q11" s="240"/>
-      <c r="R11" s="3"/>
+      <c r="R11" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="S11" s="4" t="s">
         <v>24</v>
       </c>
@@ -10625,7 +9376,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
-      <c r="H12" s="363"/>
+      <c r="H12" s="326"/>
       <c r="I12" s="202"/>
       <c r="J12" s="241"/>
       <c r="K12" s="238"/>
@@ -10645,7 +9396,9 @@
         <v>0</v>
       </c>
       <c r="Q12" s="242"/>
-      <c r="R12" s="3"/>
+      <c r="R12" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="S12" s="4" t="s">
         <v>25</v>
       </c>
@@ -10665,7 +9418,7 @@
       <c r="E13" s="9"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="363"/>
+      <c r="H13" s="326"/>
       <c r="I13" s="202"/>
       <c r="J13" s="241"/>
       <c r="K13" s="238"/>
@@ -10705,7 +9458,7 @@
       <c r="E14" s="9"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
-      <c r="H14" s="363"/>
+      <c r="H14" s="326"/>
       <c r="I14" s="202"/>
       <c r="J14" s="241"/>
       <c r="K14" s="238"/>
@@ -10745,7 +9498,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
-      <c r="H15" s="363"/>
+      <c r="H15" s="326"/>
       <c r="I15" s="202"/>
       <c r="J15" s="241"/>
       <c r="K15" s="238"/>
@@ -10783,7 +9536,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
-      <c r="H16" s="363"/>
+      <c r="H16" s="326"/>
       <c r="I16" s="202"/>
       <c r="J16" s="52"/>
       <c r="K16" s="59"/>
@@ -10819,7 +9572,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="363"/>
+      <c r="H17" s="326"/>
       <c r="I17" s="202"/>
       <c r="J17" s="241"/>
       <c r="K17" s="59"/>
@@ -10855,7 +9608,7 @@
       <c r="E18" s="9"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="363"/>
+      <c r="H18" s="326"/>
       <c r="I18" s="202"/>
       <c r="J18" s="52"/>
       <c r="K18" s="59"/>
@@ -10891,7 +9644,7 @@
       <c r="E19" s="9"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="363"/>
+      <c r="H19" s="326"/>
       <c r="I19" s="202"/>
       <c r="J19" s="241"/>
       <c r="K19" s="238"/>
@@ -10927,7 +9680,7 @@
       <c r="E20" s="9"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="363"/>
+      <c r="H20" s="326"/>
       <c r="I20" s="202"/>
       <c r="J20" s="241"/>
       <c r="K20" s="238"/>
@@ -10963,7 +9716,7 @@
       <c r="E21" s="9"/>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="363"/>
+      <c r="H21" s="326"/>
       <c r="I21" s="202"/>
       <c r="J21" s="52"/>
       <c r="K21" s="59"/>
@@ -10999,7 +9752,7 @@
       <c r="E22" s="9"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="363"/>
+      <c r="H22" s="326"/>
       <c r="I22" s="202"/>
       <c r="J22" s="241"/>
       <c r="K22" s="59"/>
@@ -11035,7 +9788,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
-      <c r="H23" s="363"/>
+      <c r="H23" s="326"/>
       <c r="I23" s="202"/>
       <c r="J23" s="241"/>
       <c r="K23" s="238"/>
@@ -11071,7 +9824,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="363"/>
+      <c r="H24" s="326"/>
       <c r="I24" s="202"/>
       <c r="J24" s="241"/>
       <c r="K24" s="238"/>
@@ -11107,7 +9860,7 @@
       <c r="E25" s="9"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="363"/>
+      <c r="H25" s="326"/>
       <c r="I25" s="202"/>
       <c r="J25" s="241"/>
       <c r="K25" s="238"/>
@@ -11143,7 +9896,7 @@
       <c r="E26" s="9"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
-      <c r="H26" s="363"/>
+      <c r="H26" s="326"/>
       <c r="I26" s="202"/>
       <c r="J26" s="52"/>
       <c r="K26" s="59"/>
@@ -11179,7 +9932,7 @@
       <c r="E27" s="9"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
-      <c r="H27" s="363"/>
+      <c r="H27" s="326"/>
       <c r="I27" s="202"/>
       <c r="J27" s="241"/>
       <c r="K27" s="239"/>
@@ -11215,7 +9968,7 @@
       <c r="E28" s="9"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
-      <c r="H28" s="363"/>
+      <c r="H28" s="326"/>
       <c r="I28" s="202"/>
       <c r="J28" s="241"/>
       <c r="K28" s="238"/>
@@ -11251,7 +10004,7 @@
       <c r="E29" s="9"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
-      <c r="H29" s="363"/>
+      <c r="H29" s="326"/>
       <c r="I29" s="202"/>
       <c r="J29" s="241"/>
       <c r="K29" s="238"/>
@@ -11287,7 +10040,7 @@
       <c r="E30" s="9"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
-      <c r="H30" s="363"/>
+      <c r="H30" s="326"/>
       <c r="I30" s="202"/>
       <c r="J30" s="241"/>
       <c r="K30" s="238"/>
@@ -11323,7 +10076,7 @@
       <c r="E31" s="9"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
-      <c r="H31" s="363"/>
+      <c r="H31" s="326"/>
       <c r="I31" s="202"/>
       <c r="J31" s="52"/>
       <c r="K31" s="59"/>
@@ -11359,7 +10112,7 @@
       <c r="E32" s="9"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
-      <c r="H32" s="363"/>
+      <c r="H32" s="326"/>
       <c r="I32" s="202"/>
       <c r="J32" s="241"/>
       <c r="K32" s="59"/>
@@ -11395,7 +10148,7 @@
       <c r="E33" s="9"/>
       <c r="F33" s="22"/>
       <c r="G33" s="22"/>
-      <c r="H33" s="363"/>
+      <c r="H33" s="326"/>
       <c r="I33" s="202"/>
       <c r="J33" s="241"/>
       <c r="K33" s="238"/>
@@ -11431,7 +10184,7 @@
       <c r="E34" s="9"/>
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
-      <c r="H34" s="363"/>
+      <c r="H34" s="326"/>
       <c r="I34" s="202"/>
       <c r="J34" s="241"/>
       <c r="K34" s="238"/>
@@ -11467,7 +10220,7 @@
       <c r="E35" s="16"/>
       <c r="F35" s="70"/>
       <c r="G35" s="70"/>
-      <c r="H35" s="363"/>
+      <c r="H35" s="326"/>
       <c r="I35" s="202"/>
       <c r="J35" s="52"/>
       <c r="K35" s="67"/>
@@ -11503,7 +10256,7 @@
       <c r="E36" s="9"/>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
-      <c r="H36" s="363"/>
+      <c r="H36" s="326"/>
       <c r="I36" s="202"/>
       <c r="J36" s="241"/>
       <c r="K36" s="59"/>
@@ -11539,7 +10292,7 @@
       <c r="E37" s="9"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
-      <c r="H37" s="363"/>
+      <c r="H37" s="326"/>
       <c r="I37" s="202"/>
       <c r="J37" s="241"/>
       <c r="K37" s="238"/>
@@ -11575,7 +10328,7 @@
       <c r="E38" s="10"/>
       <c r="F38" s="41"/>
       <c r="G38" s="41"/>
-      <c r="H38" s="363"/>
+      <c r="H38" s="326"/>
       <c r="I38" s="202"/>
       <c r="J38" s="52"/>
       <c r="K38" s="238"/>
@@ -11611,7 +10364,7 @@
       <c r="E39" s="9"/>
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
-      <c r="H39" s="363"/>
+      <c r="H39" s="326"/>
       <c r="I39" s="202"/>
       <c r="J39" s="52"/>
       <c r="K39" s="238"/>
@@ -11647,7 +10400,7 @@
       <c r="E40" s="9"/>
       <c r="F40" s="22"/>
       <c r="G40" s="22"/>
-      <c r="H40" s="363"/>
+      <c r="H40" s="326"/>
       <c r="I40" s="202"/>
       <c r="J40" s="52"/>
       <c r="K40" s="238"/>
@@ -11683,7 +10436,7 @@
       <c r="E41" s="9"/>
       <c r="F41" s="22"/>
       <c r="G41" s="22"/>
-      <c r="H41" s="363"/>
+      <c r="H41" s="326"/>
       <c r="I41" s="202"/>
       <c r="J41" s="52"/>
       <c r="K41" s="238"/>
@@ -11719,7 +10472,7 @@
       <c r="E42" s="9"/>
       <c r="F42" s="22"/>
       <c r="G42" s="22"/>
-      <c r="H42" s="363"/>
+      <c r="H42" s="326"/>
       <c r="I42" s="202"/>
       <c r="J42" s="52"/>
       <c r="K42" s="238"/>
@@ -11755,7 +10508,7 @@
       <c r="E43" s="9"/>
       <c r="F43" s="22"/>
       <c r="G43" s="22"/>
-      <c r="H43" s="363"/>
+      <c r="H43" s="326"/>
       <c r="I43" s="202"/>
       <c r="J43" s="52"/>
       <c r="K43" s="238"/>
@@ -11791,7 +10544,7 @@
       <c r="E44" s="10"/>
       <c r="F44" s="74"/>
       <c r="G44" s="74"/>
-      <c r="H44" s="365"/>
+      <c r="H44" s="328"/>
       <c r="I44" s="244"/>
       <c r="J44" s="21"/>
       <c r="K44" s="130"/>
@@ -12002,32 +10755,32 @@
       <c r="X50" s="198"/>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="331" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="332"/>
-      <c r="C51" s="332"/>
-      <c r="D51" s="332"/>
-      <c r="E51" s="332"/>
-      <c r="F51" s="332"/>
-      <c r="G51" s="332"/>
-      <c r="H51" s="332"/>
-      <c r="I51" s="332"/>
-      <c r="J51" s="332"/>
-      <c r="K51" s="332"/>
-      <c r="L51" s="332"/>
-      <c r="M51" s="332"/>
-      <c r="N51" s="332"/>
-      <c r="O51" s="332"/>
-      <c r="P51" s="332"/>
-      <c r="Q51" s="332"/>
-      <c r="R51" s="332"/>
-      <c r="S51" s="332"/>
-      <c r="T51" s="332"/>
-      <c r="U51" s="332"/>
-      <c r="V51" s="332"/>
-      <c r="W51" s="332"/>
-      <c r="X51" s="333"/>
+      <c r="A51" s="345" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="346"/>
+      <c r="C51" s="346"/>
+      <c r="D51" s="346"/>
+      <c r="E51" s="346"/>
+      <c r="F51" s="346"/>
+      <c r="G51" s="346"/>
+      <c r="H51" s="346"/>
+      <c r="I51" s="346"/>
+      <c r="J51" s="346"/>
+      <c r="K51" s="346"/>
+      <c r="L51" s="346"/>
+      <c r="M51" s="346"/>
+      <c r="N51" s="346"/>
+      <c r="O51" s="346"/>
+      <c r="P51" s="346"/>
+      <c r="Q51" s="346"/>
+      <c r="R51" s="346"/>
+      <c r="S51" s="346"/>
+      <c r="T51" s="346"/>
+      <c r="U51" s="346"/>
+      <c r="V51" s="346"/>
+      <c r="W51" s="346"/>
+      <c r="X51" s="347"/>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="336" t="s">
@@ -12058,9 +10811,9 @@
       <c r="X52" s="338"/>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="339"/>
-      <c r="B53" s="340"/>
-      <c r="C53" s="340"/>
+      <c r="A53" s="350"/>
+      <c r="B53" s="351"/>
+      <c r="C53" s="351"/>
       <c r="D53" s="224"/>
       <c r="E53" s="224"/>
       <c r="F53" s="224"/>
@@ -12086,52 +10839,52 @@
       </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" s="341"/>
-      <c r="B54" s="342"/>
-      <c r="C54" s="342"/>
-      <c r="D54" s="342"/>
-      <c r="E54" s="342"/>
-      <c r="F54" s="342"/>
-      <c r="G54" s="342"/>
-      <c r="H54" s="342"/>
-      <c r="I54" s="342"/>
-      <c r="J54" s="342"/>
-      <c r="K54" s="342"/>
-      <c r="L54" s="342"/>
-      <c r="M54" s="342"/>
-      <c r="N54" s="342"/>
-      <c r="O54" s="342"/>
-      <c r="P54" s="342"/>
-      <c r="Q54" s="342"/>
-      <c r="R54" s="342"/>
-      <c r="S54" s="342"/>
-      <c r="T54" s="342"/>
-      <c r="U54" s="342"/>
-      <c r="V54" s="342"/>
-      <c r="W54" s="342"/>
-      <c r="X54" s="343"/>
+      <c r="A54" s="352"/>
+      <c r="B54" s="353"/>
+      <c r="C54" s="353"/>
+      <c r="D54" s="353"/>
+      <c r="E54" s="353"/>
+      <c r="F54" s="353"/>
+      <c r="G54" s="353"/>
+      <c r="H54" s="353"/>
+      <c r="I54" s="353"/>
+      <c r="J54" s="353"/>
+      <c r="K54" s="353"/>
+      <c r="L54" s="353"/>
+      <c r="M54" s="353"/>
+      <c r="N54" s="353"/>
+      <c r="O54" s="353"/>
+      <c r="P54" s="353"/>
+      <c r="Q54" s="353"/>
+      <c r="R54" s="353"/>
+      <c r="S54" s="353"/>
+      <c r="T54" s="353"/>
+      <c r="U54" s="353"/>
+      <c r="V54" s="353"/>
+      <c r="W54" s="353"/>
+      <c r="X54" s="354"/>
     </row>
     <row r="55" spans="1:24" ht="59.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="344"/>
-      <c r="B55" s="345"/>
-      <c r="C55" s="345"/>
-      <c r="D55" s="345"/>
-      <c r="E55" s="345"/>
-      <c r="F55" s="345"/>
-      <c r="G55" s="345"/>
-      <c r="H55" s="345"/>
-      <c r="I55" s="345"/>
-      <c r="J55" s="345"/>
-      <c r="K55" s="345"/>
-      <c r="L55" s="345"/>
-      <c r="M55" s="345"/>
-      <c r="N55" s="345"/>
-      <c r="O55" s="345"/>
-      <c r="P55" s="345"/>
-      <c r="Q55" s="345"/>
-      <c r="R55" s="345"/>
-      <c r="S55" s="345"/>
-      <c r="T55" s="345"/>
+      <c r="A55" s="355"/>
+      <c r="B55" s="356"/>
+      <c r="C55" s="356"/>
+      <c r="D55" s="356"/>
+      <c r="E55" s="356"/>
+      <c r="F55" s="356"/>
+      <c r="G55" s="356"/>
+      <c r="H55" s="356"/>
+      <c r="I55" s="356"/>
+      <c r="J55" s="356"/>
+      <c r="K55" s="356"/>
+      <c r="L55" s="356"/>
+      <c r="M55" s="356"/>
+      <c r="N55" s="356"/>
+      <c r="O55" s="356"/>
+      <c r="P55" s="356"/>
+      <c r="Q55" s="356"/>
+      <c r="R55" s="356"/>
+      <c r="S55" s="356"/>
+      <c r="T55" s="356"/>
       <c r="U55" s="314" t="s">
         <v>78</v>
       </c>
@@ -12173,27 +10926,27 @@
       <c r="A57" s="106"/>
       <c r="B57" s="107"/>
       <c r="C57" s="108"/>
-      <c r="D57" s="326" t="s">
+      <c r="D57" s="357" t="s">
         <v>7</v>
       </c>
-      <c r="E57" s="327"/>
-      <c r="F57" s="327"/>
-      <c r="G57" s="327"/>
-      <c r="H57" s="327"/>
-      <c r="I57" s="327"/>
-      <c r="J57" s="328"/>
-      <c r="K57" s="356" t="s">
+      <c r="E57" s="358"/>
+      <c r="F57" s="358"/>
+      <c r="G57" s="358"/>
+      <c r="H57" s="358"/>
+      <c r="I57" s="358"/>
+      <c r="J57" s="359"/>
+      <c r="K57" s="360" t="s">
         <v>8</v>
       </c>
-      <c r="L57" s="357"/>
-      <c r="M57" s="356" t="s">
+      <c r="L57" s="361"/>
+      <c r="M57" s="360" t="s">
         <v>9</v>
       </c>
-      <c r="N57" s="357"/>
-      <c r="O57" s="326" t="s">
+      <c r="N57" s="361"/>
+      <c r="O57" s="357" t="s">
         <v>10</v>
       </c>
-      <c r="P57" s="328"/>
+      <c r="P57" s="359"/>
       <c r="Q57" s="109"/>
       <c r="R57" s="107"/>
       <c r="S57" s="109"/>
@@ -12223,10 +10976,10 @@
       <c r="G58" s="113" t="s">
         <v>64</v>
       </c>
-      <c r="H58" s="358" t="s">
+      <c r="H58" s="362" t="s">
         <v>15</v>
       </c>
-      <c r="I58" s="359"/>
+      <c r="I58" s="363"/>
       <c r="J58" s="114" t="s">
         <v>16</v>
       </c>
@@ -12275,10 +11028,10 @@
       <c r="G59" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="H59" s="360" t="s">
+      <c r="H59" s="364" t="s">
         <v>20</v>
       </c>
-      <c r="I59" s="361"/>
+      <c r="I59" s="365"/>
       <c r="J59" s="122" t="s">
         <v>21</v>
       </c>
@@ -12295,7 +11048,9 @@
         <v>21</v>
       </c>
       <c r="Q59" s="120"/>
-      <c r="R59" s="80"/>
+      <c r="R59" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="S59" s="11" t="s">
         <v>22</v>
       </c>
@@ -12313,7 +11068,7 @@
       <c r="E60" s="33"/>
       <c r="F60" s="84"/>
       <c r="G60" s="75"/>
-      <c r="H60" s="362"/>
+      <c r="H60" s="325"/>
       <c r="I60" s="232"/>
       <c r="J60" s="233"/>
       <c r="K60" s="238"/>
@@ -12333,7 +11088,9 @@
         <v>0</v>
       </c>
       <c r="Q60" s="235"/>
-      <c r="R60" s="80"/>
+      <c r="R60" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="S60" s="11" t="s">
         <v>23</v>
       </c>
@@ -12351,7 +11108,7 @@
       <c r="E61" s="9"/>
       <c r="F61" s="22"/>
       <c r="G61" s="22"/>
-      <c r="H61" s="363"/>
+      <c r="H61" s="326"/>
       <c r="I61" s="202"/>
       <c r="J61" s="52"/>
       <c r="K61" s="238"/>
@@ -12371,7 +11128,9 @@
         <v>0</v>
       </c>
       <c r="Q61" s="242"/>
-      <c r="R61" s="3"/>
+      <c r="R61" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="S61" s="4" t="s">
         <v>24</v>
       </c>
@@ -12389,7 +11148,7 @@
       <c r="E62" s="10"/>
       <c r="F62" s="41"/>
       <c r="G62" s="41"/>
-      <c r="H62" s="363"/>
+      <c r="H62" s="326"/>
       <c r="I62" s="202"/>
       <c r="J62" s="241"/>
       <c r="K62" s="238"/>
@@ -12409,7 +11168,9 @@
         <v>0</v>
       </c>
       <c r="Q62" s="242"/>
-      <c r="R62" s="3"/>
+      <c r="R62" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="S62" s="4" t="s">
         <v>25</v>
       </c>
@@ -12429,7 +11190,7 @@
       <c r="E63" s="10"/>
       <c r="F63" s="41"/>
       <c r="G63" s="41"/>
-      <c r="H63" s="363"/>
+      <c r="H63" s="326"/>
       <c r="I63" s="202"/>
       <c r="J63" s="241"/>
       <c r="K63" s="238"/>
@@ -12453,9 +11214,9 @@
       <c r="S63" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="T63" s="334"/>
-      <c r="U63" s="334"/>
-      <c r="V63" s="334"/>
+      <c r="T63" s="348"/>
+      <c r="U63" s="348"/>
+      <c r="V63" s="348"/>
       <c r="W63" s="4" t="s">
         <v>28</v>
       </c>
@@ -12469,7 +11230,7 @@
       <c r="E64" s="10"/>
       <c r="F64" s="41"/>
       <c r="G64" s="41"/>
-      <c r="H64" s="363"/>
+      <c r="H64" s="326"/>
       <c r="I64" s="202"/>
       <c r="J64" s="52"/>
       <c r="K64" s="238"/>
@@ -12491,12 +11252,12 @@
       <c r="Q64" s="242"/>
       <c r="R64" s="83"/>
       <c r="S64" s="47"/>
-      <c r="T64" s="335" t="str">
+      <c r="T64" s="349" t="str">
         <f>+T14</f>
         <v>( นาย... )</v>
       </c>
-      <c r="U64" s="335"/>
-      <c r="V64" s="335"/>
+      <c r="U64" s="349"/>
+      <c r="V64" s="349"/>
       <c r="W64" s="4" t="s">
         <v>29</v>
       </c>
@@ -12510,7 +11271,7 @@
       <c r="E65" s="10"/>
       <c r="F65" s="41"/>
       <c r="G65" s="41"/>
-      <c r="H65" s="363"/>
+      <c r="H65" s="326"/>
       <c r="I65" s="202"/>
       <c r="J65" s="52"/>
       <c r="K65" s="238"/>
@@ -12548,7 +11309,7 @@
       <c r="E66" s="9"/>
       <c r="F66" s="22"/>
       <c r="G66" s="22"/>
-      <c r="H66" s="363"/>
+      <c r="H66" s="326"/>
       <c r="I66" s="202"/>
       <c r="J66" s="52"/>
       <c r="K66" s="238"/>
@@ -12584,7 +11345,7 @@
       <c r="E67" s="9"/>
       <c r="F67" s="22"/>
       <c r="G67" s="22"/>
-      <c r="H67" s="363"/>
+      <c r="H67" s="326"/>
       <c r="I67" s="202"/>
       <c r="J67" s="237"/>
       <c r="K67" s="238"/>
@@ -12622,7 +11383,7 @@
       <c r="E68" s="9"/>
       <c r="F68" s="22"/>
       <c r="G68" s="22"/>
-      <c r="H68" s="363"/>
+      <c r="H68" s="326"/>
       <c r="I68" s="202"/>
       <c r="J68" s="52"/>
       <c r="K68" s="238"/>
@@ -12660,7 +11421,7 @@
       <c r="E69" s="10"/>
       <c r="F69" s="41"/>
       <c r="G69" s="41"/>
-      <c r="H69" s="363"/>
+      <c r="H69" s="326"/>
       <c r="I69" s="202"/>
       <c r="J69" s="237"/>
       <c r="K69" s="238"/>
@@ -12700,7 +11461,7 @@
       <c r="E70" s="10"/>
       <c r="F70" s="41"/>
       <c r="G70" s="41"/>
-      <c r="H70" s="363"/>
+      <c r="H70" s="326"/>
       <c r="I70" s="202"/>
       <c r="J70" s="52"/>
       <c r="K70" s="238"/>
@@ -12720,7 +11481,9 @@
         <v>0</v>
       </c>
       <c r="Q70" s="242"/>
-      <c r="R70" s="3"/>
+      <c r="R70" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="S70" s="4" t="s">
         <v>41</v>
       </c>
@@ -12738,7 +11501,7 @@
       <c r="E71" s="10"/>
       <c r="F71" s="41"/>
       <c r="G71" s="41"/>
-      <c r="H71" s="363"/>
+      <c r="H71" s="326"/>
       <c r="I71" s="202"/>
       <c r="J71" s="52"/>
       <c r="K71" s="238"/>
@@ -12758,7 +11521,9 @@
         <v>0</v>
       </c>
       <c r="Q71" s="242"/>
-      <c r="R71" s="3"/>
+      <c r="R71" s="366" t="s">
+        <v>79</v>
+      </c>
       <c r="S71" s="4" t="s">
         <v>42</v>
       </c>
@@ -12776,7 +11541,7 @@
       <c r="E72" s="72"/>
       <c r="F72" s="76"/>
       <c r="G72" s="76"/>
-      <c r="H72" s="363"/>
+      <c r="H72" s="326"/>
       <c r="I72" s="202"/>
       <c r="J72" s="236"/>
       <c r="K72" s="238"/>
@@ -12814,7 +11579,7 @@
       <c r="E73" s="10"/>
       <c r="F73" s="41"/>
       <c r="G73" s="41"/>
-      <c r="H73" s="363"/>
+      <c r="H73" s="326"/>
       <c r="I73" s="202"/>
       <c r="J73" s="241"/>
       <c r="K73" s="238"/>
@@ -12852,7 +11617,7 @@
       <c r="E74" s="10"/>
       <c r="F74" s="41"/>
       <c r="G74" s="41"/>
-      <c r="H74" s="363"/>
+      <c r="H74" s="326"/>
       <c r="I74" s="202"/>
       <c r="J74" s="241"/>
       <c r="K74" s="238"/>
@@ -12895,7 +11660,7 @@
       <c r="E75" s="10"/>
       <c r="F75" s="41"/>
       <c r="G75" s="41"/>
-      <c r="H75" s="363"/>
+      <c r="H75" s="326"/>
       <c r="I75" s="202"/>
       <c r="J75" s="52"/>
       <c r="K75" s="238"/>
@@ -12938,7 +11703,7 @@
       <c r="E76" s="9"/>
       <c r="F76" s="22"/>
       <c r="G76" s="22"/>
-      <c r="H76" s="363"/>
+      <c r="H76" s="326"/>
       <c r="I76" s="202"/>
       <c r="J76" s="236"/>
       <c r="K76" s="238"/>
@@ -12980,7 +11745,7 @@
       <c r="E77" s="9"/>
       <c r="F77" s="22"/>
       <c r="G77" s="22"/>
-      <c r="H77" s="363"/>
+      <c r="H77" s="326"/>
       <c r="I77" s="202"/>
       <c r="J77" s="236"/>
       <c r="K77" s="238"/>
@@ -13023,7 +11788,7 @@
       <c r="E78" s="9"/>
       <c r="F78" s="22"/>
       <c r="G78" s="22"/>
-      <c r="H78" s="363"/>
+      <c r="H78" s="326"/>
       <c r="I78" s="202"/>
       <c r="J78" s="236"/>
       <c r="K78" s="238"/>
@@ -13066,7 +11831,7 @@
       <c r="E79" s="9"/>
       <c r="F79" s="22"/>
       <c r="G79" s="22"/>
-      <c r="H79" s="363"/>
+      <c r="H79" s="326"/>
       <c r="I79" s="202"/>
       <c r="J79" s="236"/>
       <c r="K79" s="238"/>
@@ -13109,7 +11874,7 @@
       <c r="E80" s="26"/>
       <c r="F80" s="9"/>
       <c r="G80" s="77"/>
-      <c r="H80" s="363"/>
+      <c r="H80" s="326"/>
       <c r="I80" s="202"/>
       <c r="J80" s="53"/>
       <c r="K80" s="52"/>
@@ -13153,7 +11918,7 @@
       <c r="E81" s="26"/>
       <c r="F81" s="9"/>
       <c r="G81" s="77"/>
-      <c r="H81" s="363"/>
+      <c r="H81" s="326"/>
       <c r="I81" s="202"/>
       <c r="J81" s="52"/>
       <c r="K81" s="52"/>
@@ -13195,7 +11960,7 @@
       <c r="E82" s="10"/>
       <c r="F82" s="41"/>
       <c r="G82" s="41"/>
-      <c r="H82" s="363"/>
+      <c r="H82" s="326"/>
       <c r="I82" s="202"/>
       <c r="J82" s="52"/>
       <c r="K82" s="52"/>
@@ -13237,7 +12002,7 @@
       <c r="E83" s="10"/>
       <c r="F83" s="41"/>
       <c r="G83" s="41"/>
-      <c r="H83" s="363"/>
+      <c r="H83" s="326"/>
       <c r="I83" s="202"/>
       <c r="J83" s="52"/>
       <c r="K83" s="52"/>
@@ -13279,7 +12044,7 @@
       <c r="E84" s="10"/>
       <c r="F84" s="41"/>
       <c r="G84" s="41"/>
-      <c r="H84" s="363"/>
+      <c r="H84" s="326"/>
       <c r="I84" s="202"/>
       <c r="J84" s="52"/>
       <c r="K84" s="52"/>
@@ -13322,7 +12087,7 @@
       <c r="E85" s="13"/>
       <c r="F85" s="78"/>
       <c r="G85" s="78"/>
-      <c r="H85" s="363"/>
+      <c r="H85" s="326"/>
       <c r="I85" s="202"/>
       <c r="J85" s="52"/>
       <c r="K85" s="52"/>
@@ -13361,7 +12126,7 @@
       <c r="E86" s="10"/>
       <c r="F86" s="41"/>
       <c r="G86" s="41"/>
-      <c r="H86" s="363"/>
+      <c r="H86" s="326"/>
       <c r="I86" s="202"/>
       <c r="J86" s="52"/>
       <c r="K86" s="52"/>
@@ -13397,7 +12162,7 @@
       <c r="E87" s="10"/>
       <c r="F87" s="41"/>
       <c r="G87" s="41"/>
-      <c r="H87" s="363"/>
+      <c r="H87" s="326"/>
       <c r="I87" s="202"/>
       <c r="J87" s="52"/>
       <c r="K87" s="52"/>
@@ -13433,7 +12198,7 @@
       <c r="E88" s="10"/>
       <c r="F88" s="41"/>
       <c r="G88" s="41"/>
-      <c r="H88" s="363"/>
+      <c r="H88" s="326"/>
       <c r="I88" s="202"/>
       <c r="J88" s="52"/>
       <c r="K88" s="52"/>
@@ -13469,7 +12234,7 @@
       <c r="E89" s="10"/>
       <c r="F89" s="41"/>
       <c r="G89" s="41"/>
-      <c r="H89" s="363"/>
+      <c r="H89" s="326"/>
       <c r="I89" s="202"/>
       <c r="J89" s="52"/>
       <c r="K89" s="52"/>
@@ -13505,7 +12270,7 @@
       <c r="E90" s="10"/>
       <c r="F90" s="41"/>
       <c r="G90" s="41"/>
-      <c r="H90" s="363"/>
+      <c r="H90" s="326"/>
       <c r="I90" s="202"/>
       <c r="J90" s="52"/>
       <c r="K90" s="52"/>
@@ -13541,7 +12306,7 @@
       <c r="E91" s="10"/>
       <c r="F91" s="41"/>
       <c r="G91" s="41"/>
-      <c r="H91" s="363"/>
+      <c r="H91" s="326"/>
       <c r="I91" s="202"/>
       <c r="J91" s="52"/>
       <c r="K91" s="52"/>
@@ -13577,7 +12342,7 @@
       <c r="E92" s="10"/>
       <c r="F92" s="41"/>
       <c r="G92" s="41"/>
-      <c r="H92" s="363"/>
+      <c r="H92" s="326"/>
       <c r="I92" s="202"/>
       <c r="J92" s="52"/>
       <c r="K92" s="52"/>
@@ -13613,7 +12378,7 @@
       <c r="E93" s="13"/>
       <c r="F93" s="78"/>
       <c r="G93" s="78"/>
-      <c r="H93" s="363"/>
+      <c r="H93" s="326"/>
       <c r="I93" s="202"/>
       <c r="J93" s="52"/>
       <c r="K93" s="52"/>
@@ -13649,7 +12414,7 @@
       <c r="E94" s="10"/>
       <c r="F94" s="74"/>
       <c r="G94" s="74"/>
-      <c r="H94" s="364"/>
+      <c r="H94" s="327"/>
       <c r="I94" s="248"/>
       <c r="J94" s="52"/>
       <c r="K94" s="52"/>
@@ -13679,10 +12444,10 @@
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="151"/>
-      <c r="B95" s="329" t="s">
+      <c r="B95" s="343" t="s">
         <v>37</v>
       </c>
-      <c r="C95" s="330"/>
+      <c r="C95" s="344"/>
       <c r="D95" s="154"/>
       <c r="E95" s="155"/>
       <c r="F95" s="155"/>
@@ -13751,15 +12516,15 @@
         <v>0</v>
       </c>
       <c r="Q96" s="160"/>
-      <c r="R96" s="350" t="s">
+      <c r="R96" s="333" t="s">
         <v>59</v>
       </c>
-      <c r="S96" s="351"/>
-      <c r="T96" s="351"/>
-      <c r="U96" s="351"/>
-      <c r="V96" s="351"/>
-      <c r="W96" s="351"/>
-      <c r="X96" s="352"/>
+      <c r="S96" s="334"/>
+      <c r="T96" s="334"/>
+      <c r="U96" s="334"/>
+      <c r="V96" s="334"/>
+      <c r="W96" s="334"/>
+      <c r="X96" s="335"/>
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="336" t="s">
@@ -13796,9 +12561,9 @@
       <c r="X97" s="185"/>
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" s="353"/>
-      <c r="B98" s="346"/>
-      <c r="C98" s="354"/>
+      <c r="A98" s="340"/>
+      <c r="B98" s="329"/>
+      <c r="C98" s="341"/>
       <c r="D98" s="179"/>
       <c r="E98" s="179"/>
       <c r="F98" s="179"/>
@@ -13826,22 +12591,22 @@
       <c r="X98" s="185"/>
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="353" t="s">
+      <c r="A99" s="340" t="s">
         <v>33</v>
       </c>
-      <c r="B99" s="346"/>
-      <c r="C99" s="354"/>
+      <c r="B99" s="329"/>
+      <c r="C99" s="341"/>
       <c r="D99" s="4"/>
-      <c r="E99" s="355" t="s">
+      <c r="E99" s="342" t="s">
         <v>34</v>
       </c>
-      <c r="F99" s="355"/>
-      <c r="G99" s="355"/>
-      <c r="H99" s="355"/>
-      <c r="I99" s="355"/>
-      <c r="J99" s="355"/>
-      <c r="K99" s="355"/>
-      <c r="L99" s="355"/>
+      <c r="F99" s="342"/>
+      <c r="G99" s="342"/>
+      <c r="H99" s="342"/>
+      <c r="I99" s="342"/>
+      <c r="J99" s="342"/>
+      <c r="K99" s="342"/>
+      <c r="L99" s="342"/>
       <c r="M99" s="181"/>
       <c r="N99" s="250"/>
       <c r="O99" s="251"/>
@@ -13858,21 +12623,21 @@
       <c r="X99" s="185"/>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A100" s="353"/>
-      <c r="B100" s="346"/>
-      <c r="C100" s="354"/>
+      <c r="A100" s="340"/>
+      <c r="B100" s="329"/>
+      <c r="C100" s="341"/>
       <c r="D100" s="4"/>
       <c r="E100" s="177"/>
-      <c r="F100" s="346" t="str">
+      <c r="F100" s="329" t="str">
         <f>+H49</f>
         <v>( นาย... ) ตำแหน่ง กบศ.</v>
       </c>
-      <c r="G100" s="346"/>
-      <c r="H100" s="346"/>
-      <c r="I100" s="346"/>
-      <c r="J100" s="346"/>
-      <c r="K100" s="346"/>
-      <c r="L100" s="346"/>
+      <c r="G100" s="329"/>
+      <c r="H100" s="329"/>
+      <c r="I100" s="329"/>
+      <c r="J100" s="329"/>
+      <c r="K100" s="329"/>
+      <c r="L100" s="329"/>
       <c r="M100" s="254"/>
       <c r="N100" s="255"/>
       <c r="O100" s="256"/>
@@ -13891,22 +12656,22 @@
       <c r="X100" s="217"/>
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="347" t="s">
+      <c r="A101" s="330" t="s">
         <v>35</v>
       </c>
-      <c r="B101" s="348"/>
-      <c r="C101" s="349"/>
+      <c r="B101" s="331"/>
+      <c r="C101" s="332"/>
       <c r="D101" s="139"/>
       <c r="E101" s="87"/>
-      <c r="F101" s="348" t="s">
+      <c r="F101" s="331" t="s">
         <v>36</v>
       </c>
-      <c r="G101" s="348"/>
-      <c r="H101" s="348"/>
-      <c r="I101" s="348"/>
-      <c r="J101" s="348"/>
-      <c r="K101" s="348"/>
-      <c r="L101" s="348"/>
+      <c r="G101" s="331"/>
+      <c r="H101" s="331"/>
+      <c r="I101" s="331"/>
+      <c r="J101" s="331"/>
+      <c r="K101" s="331"/>
+      <c r="L101" s="331"/>
       <c r="M101" s="258"/>
       <c r="N101" s="259"/>
       <c r="O101" s="260"/>
@@ -13940,22 +12705,12 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A51:X51"/>
-    <mergeCell ref="A52:X52"/>
-    <mergeCell ref="A54:X54"/>
-    <mergeCell ref="D57:J57"/>
-    <mergeCell ref="K57:L57"/>
-    <mergeCell ref="M57:N57"/>
-    <mergeCell ref="O57:P57"/>
-    <mergeCell ref="A55:T55"/>
+    <mergeCell ref="A99:C99"/>
+    <mergeCell ref="E99:L99"/>
+    <mergeCell ref="A100:C100"/>
+    <mergeCell ref="A101:C101"/>
+    <mergeCell ref="F100:L100"/>
+    <mergeCell ref="F101:L101"/>
     <mergeCell ref="A98:C98"/>
     <mergeCell ref="H58:I58"/>
     <mergeCell ref="H59:I59"/>
@@ -13964,18 +12719,27 @@
     <mergeCell ref="B95:C95"/>
     <mergeCell ref="R96:X96"/>
     <mergeCell ref="A97:C97"/>
-    <mergeCell ref="A99:C99"/>
-    <mergeCell ref="E99:L99"/>
-    <mergeCell ref="A100:C100"/>
-    <mergeCell ref="A101:C101"/>
-    <mergeCell ref="F100:L100"/>
-    <mergeCell ref="F101:L101"/>
+    <mergeCell ref="A54:X54"/>
+    <mergeCell ref="D57:J57"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="M57:N57"/>
+    <mergeCell ref="O57:P57"/>
+    <mergeCell ref="A55:T55"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A51:X51"/>
+    <mergeCell ref="A52:X52"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" scale="28" fitToHeight="2" orientation="landscape" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="50" max="16383" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>